<commit_message>
can assign conduction index
</commit_message>
<xml_diff>
--- a/input/template/RGF_template.xlsx
+++ b/input/template/RGF_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="manual" sheetId="3" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>isRGF</t>
   </si>
   <si>
-    <t>Graphene</t>
-  </si>
-  <si>
     <t>MLG</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -78,9 +75,6 @@
     <t>Armchair</t>
   </si>
   <si>
-    <t>AGNR</t>
-  </si>
-  <si>
     <t>enable</t>
   </si>
   <si>
@@ -261,6 +255,14 @@
   </si>
   <si>
     <t>wave</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoS2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMNR</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -333,12 +335,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -625,7 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -635,193 +637,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>48</v>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>49</v>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>49</v>
+      <c r="B4" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>50</v>
+      <c r="B5" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>51</v>
+      <c r="B6" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>52</v>
+      <c r="B7" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>53</v>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>54</v>
+      <c r="B9" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>55</v>
+      <c r="B10" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>56</v>
+      <c r="B11" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>57</v>
+      <c r="B12" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>55</v>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>58</v>
+      <c r="B14" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>58</v>
+      <c r="B15" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>49</v>
+      <c r="B16" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>60</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -832,13 +834,13 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>62</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -849,34 +851,34 @@
     </row>
     <row r="20" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>64</v>
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="O20" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="O20" s="3"/>
     </row>
     <row r="21" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
         <v>0</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -884,45 +886,45 @@
     </row>
     <row r="22" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
         <v>5</v>
       </c>
-      <c r="H22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="P22" s="4"/>
+      <c r="H22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
         <v>1400</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
         <v>-0.03</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
         <v>-0.03</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
         <v>0.16</v>
       </c>
     </row>
@@ -942,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1009,16 +1011,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="I2" s="1">
         <v>4</v>
@@ -1039,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1060,42 +1062,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -1118,13 +1120,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D3" s="1">
         <v>5</v>
@@ -1147,13 +1149,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D4" s="1">
         <v>65</v>
@@ -1176,13 +1178,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -1205,13 +1207,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
@@ -1234,13 +1236,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D7" s="1">
         <v>65</v>

</xml_diff>